<commit_message>
before recalculating Fe rates
</commit_message>
<xml_diff>
--- a/ionrecFitSettings.xlsx
+++ b/ionrecFitSettings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmondeel/Documents/CfA/Chandra/CHANDRA-Rates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CAFDE1-8243-C340-B752-E02604BB15F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3A0701-5653-AB43-99C5-4533575E360D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1580" yWindow="4160" windowWidth="28040" windowHeight="14560" activeTab="1" xr2:uid="{70F94D0D-B77B-D34F-B605-C670112A4F1C}"/>
+    <workbookView xWindow="1580" yWindow="3640" windowWidth="28040" windowHeight="14560" activeTab="1" xr2:uid="{70F94D0D-B77B-D34F-B605-C670112A4F1C}"/>
   </bookViews>
   <sheets>
     <sheet name="O" sheetId="1" r:id="rId1"/>
@@ -840,7 +840,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1187,10 +1187,10 @@
         <v>200</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G9">
         <v>4</v>

</xml_diff>